<commit_message>
Split .xlsx input file into two separate files
</commit_message>
<xml_diff>
--- a/pairs.xlsx
+++ b/pairs.xlsx
@@ -28,28 +28,28 @@
     <t>Capitol Hillary Clinton</t>
   </si>
   <si>
+    <t>Rohni Awasthi</t>
+  </si>
+  <si>
+    <t>Larry Richards</t>
+  </si>
+  <si>
+    <t>Shirali Nigam</t>
+  </si>
+  <si>
+    <t>Parry Hotter</t>
+  </si>
+  <si>
     <t>Robyn Guarriello</t>
   </si>
   <si>
     <t>Her Mine E</t>
   </si>
   <si>
-    <t>Shirali Nigam</t>
-  </si>
-  <si>
-    <t>Parry Hotter</t>
-  </si>
-  <si>
     <t>Disha Jain</t>
   </si>
   <si>
     <t>Ron Ferretly</t>
-  </si>
-  <si>
-    <t>Rohni Awasthi</t>
-  </si>
-  <si>
-    <t>Larry Richards</t>
   </si>
   <si>
     <t>David Zhao*</t>

</xml_diff>

<commit_message>
Create a file to input file paths
Also, this commit fixes an important bug where duplicate persons referenced
the same list of preferences rather than two separate lists in memory.
</commit_message>
<xml_diff>
--- a/pairs.xlsx
+++ b/pairs.xlsx
@@ -28,40 +28,40 @@
     <t>Capitol Hillary Clinton</t>
   </si>
   <si>
+    <t>David Zhao*</t>
+  </si>
+  <si>
+    <t>Ernie and Bert Sanders</t>
+  </si>
+  <si>
+    <t>Shirali Nigam</t>
+  </si>
+  <si>
+    <t>Parry Hotter</t>
+  </si>
+  <si>
+    <t>Disha Jain</t>
+  </si>
+  <si>
+    <t>Her Mine E</t>
+  </si>
+  <si>
+    <t>Robyn Guarriello</t>
+  </si>
+  <si>
+    <t>Ben Cars- My Luggage</t>
+  </si>
+  <si>
     <t>Rohni Awasthi</t>
   </si>
   <si>
     <t>Larry Richards</t>
   </si>
   <si>
-    <t>Shirali Nigam</t>
-  </si>
-  <si>
-    <t>Parry Hotter</t>
-  </si>
-  <si>
-    <t>Robyn Guarriello</t>
-  </si>
-  <si>
-    <t>Her Mine E</t>
-  </si>
-  <si>
-    <t>Disha Jain</t>
+    <t>Disha Jain*</t>
   </si>
   <si>
     <t>Ron Ferretly</t>
-  </si>
-  <si>
-    <t>David Zhao*</t>
-  </si>
-  <si>
-    <t>Ben Cars- My Luggage</t>
-  </si>
-  <si>
-    <t>Disha Jain*</t>
-  </si>
-  <si>
-    <t>Ernie and Bert Sanders</t>
   </si>
   <si>
     <t>Robyn Guarriello*</t>

</xml_diff>

<commit_message>
Create a file to input filepaths
</commit_message>
<xml_diff>
--- a/pairs.xlsx
+++ b/pairs.xlsx
@@ -28,40 +28,40 @@
     <t>Capitol Hillary Clinton</t>
   </si>
   <si>
+    <t>David Zhao*</t>
+  </si>
+  <si>
+    <t>Ernie and Bert Sanders</t>
+  </si>
+  <si>
+    <t>Shirali Nigam</t>
+  </si>
+  <si>
+    <t>Parry Hotter</t>
+  </si>
+  <si>
+    <t>Disha Jain</t>
+  </si>
+  <si>
+    <t>Her Mine E</t>
+  </si>
+  <si>
+    <t>Robyn Guarriello</t>
+  </si>
+  <si>
+    <t>Ben Cars- My Luggage</t>
+  </si>
+  <si>
     <t>Rohni Awasthi</t>
   </si>
   <si>
     <t>Larry Richards</t>
   </si>
   <si>
-    <t>Shirali Nigam</t>
-  </si>
-  <si>
-    <t>Parry Hotter</t>
-  </si>
-  <si>
-    <t>Robyn Guarriello</t>
-  </si>
-  <si>
-    <t>Her Mine E</t>
-  </si>
-  <si>
-    <t>Disha Jain</t>
+    <t>Disha Jain*</t>
   </si>
   <si>
     <t>Ron Ferretly</t>
-  </si>
-  <si>
-    <t>David Zhao*</t>
-  </si>
-  <si>
-    <t>Ben Cars- My Luggage</t>
-  </si>
-  <si>
-    <t>Disha Jain*</t>
-  </si>
-  <si>
-    <t>Ernie and Bert Sanders</t>
   </si>
   <si>
     <t>Robyn Guarriello*</t>

</xml_diff>